<commit_message>
actualización de tiempos, Jesús
</commit_message>
<xml_diff>
--- a/planeacion/Registro_Actividades_Sistema.xlsx
+++ b/planeacion/Registro_Actividades_Sistema.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
   <si>
     <t>Actividad</t>
   </si>
@@ -82,6 +82,33 @@
   </si>
   <si>
     <t>2:00pm</t>
+  </si>
+  <si>
+    <t>Repositorio listo</t>
+  </si>
+  <si>
+    <t>Configuración de NetBeans para trabajar en el proyecto_1</t>
+  </si>
+  <si>
+    <t>6:30pm</t>
+  </si>
+  <si>
+    <t>3:00pm</t>
+  </si>
+  <si>
+    <t>Configuración de NetBeans para trabajar en el proyecto_1.1</t>
+  </si>
+  <si>
+    <t>Revisión_1</t>
+  </si>
+  <si>
+    <t>Sirio</t>
+  </si>
+  <si>
+    <t>6:00am</t>
+  </si>
+  <si>
+    <t>6:30am</t>
   </si>
 </sst>
 </file>
@@ -423,15 +450,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" customWidth="1"/>
+    <col min="1" max="1" width="54.85546875" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.85546875" customWidth="1"/>
   </cols>
@@ -572,6 +599,80 @@
       </c>
       <c r="G6" s="2">
         <v>0.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1">
+        <v>42120</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="1">
+        <v>42121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1">
+        <v>42121</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1">
+        <v>42122</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Registro de tiempos, Betty
</commit_message>
<xml_diff>
--- a/planeacion/Registro_Actividades_Sistema.xlsx
+++ b/planeacion/Registro_Actividades_Sistema.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
   <si>
     <t>Actividad</t>
   </si>
@@ -109,6 +109,18 @@
   </si>
   <si>
     <t>6:30am</t>
+  </si>
+  <si>
+    <t>Creación de la base de datos</t>
+  </si>
+  <si>
+    <t>Betty</t>
+  </si>
+  <si>
+    <t>10:45pm</t>
+  </si>
+  <si>
+    <t>11:32pm</t>
   </si>
 </sst>
 </file>
@@ -450,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,52 +638,75 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C8" s="1">
-        <v>42121</v>
+        <v>42119</v>
+      </c>
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="C9" s="1">
         <v>42121</v>
       </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0.9</v>
-      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="1">
+        <v>42121</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="1">
         <v>42122</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>29</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F11" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>